<commit_message>
adding new export features, add all data to final result
adding a much needed feature vor the programm. now you can export to pdf and generate a beautiful pdf protocol. new stats adde to protocoll bc of ezz
</commit_message>
<xml_diff>
--- a/test_data/20250918_InstrHoehe.xlsx
+++ b/test_data/20250918_InstrHoehe.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r.boppart\Documents\01_lokal_Ablage_FHNW_temp\5220_VP1\20250916_THB-Auswertung\thb-berechnung\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhnw365.sharepoint.com/teams/E-BScFeldkurs2025-VP5220GeoSensorikMonitoring_M365/Freigegebene Dokumente/Madrisa/400_GrMadrisa_Feldmessung/10_THB-Messungen/_Protokolle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D80E50C-33BF-4EE3-BBFA-69461ADA47D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="13_ncr:1_{7D80E50C-33BF-4EE3-BBFA-69461ADA47D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46991715-D799-438B-8185-AF5BD55870F3}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{C755B1BD-CD5A-4D3C-BBE6-5EE869760FAA}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{C755B1BD-CD5A-4D3C-BBE6-5EE869760FAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Visur_1003-1009</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Nr</t>
+  </si>
+  <si>
+    <t>Visur_1011-1012</t>
   </si>
 </sst>
 </file>
@@ -122,11 +125,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -142,7 +146,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -460,16 +464,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CC3F4FC-26FC-45D9-8AA4-90951A107479}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="147" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -489,247 +493,518 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>1.6803999999999999</v>
       </c>
-      <c r="D2">
-        <v>0.26819999999999999</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="1">
+        <v>0.28439999999999999</v>
+      </c>
+      <c r="E2" s="1">
         <v>1.8493999999999999</v>
       </c>
-      <c r="F2">
-        <v>0.28439999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F2" s="1">
+        <v>0.28439999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>1.6803999999999999</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
+        <v>0.28439999999999999</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2.0122</v>
+      </c>
+      <c r="F3" s="1">
         <v>0.26819999999999999</v>
       </c>
-      <c r="E3">
-        <v>2.0122</v>
-      </c>
-      <c r="F3">
-        <v>0.28439999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>1.8458000000000001</v>
       </c>
-      <c r="D4">
-        <v>0.28439999999999999</v>
-      </c>
-      <c r="E4">
+      <c r="D4" s="1">
+        <v>0.28439999999999999</v>
+      </c>
+      <c r="E4" s="1">
         <v>1.835</v>
       </c>
-      <c r="F4">
-        <v>0.28439999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F4" s="1">
+        <v>0.26819999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>1.8458000000000001</v>
       </c>
-      <c r="D5">
-        <v>0.28439999999999999</v>
-      </c>
-      <c r="E5">
-        <v>1.7844</v>
-      </c>
-      <c r="F5">
-        <v>0.26819999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D5" s="1">
+        <v>0.28439999999999999</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1.7834000000000001</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.28439999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>1.8493999999999999</v>
       </c>
-      <c r="D6">
-        <v>0.28439999999999999</v>
-      </c>
-      <c r="E6">
+      <c r="D6" s="1">
+        <v>0.28439999999999999</v>
+      </c>
+      <c r="E6" s="1">
         <v>1.5422</v>
       </c>
-      <c r="F6">
-        <v>0.28439999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F6" s="1">
+        <v>0.26819999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>1.835</v>
       </c>
-      <c r="D7">
-        <v>0.28439999999999999</v>
-      </c>
-      <c r="E7">
-        <v>1.7834000000000001</v>
-      </c>
-      <c r="F7">
+      <c r="D7" s="1">
         <v>0.26819999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E7" s="1">
+        <v>1.7844</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.28439999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>1.835</v>
       </c>
-      <c r="D8">
-        <v>0.28439999999999999</v>
-      </c>
-      <c r="E8">
+      <c r="D8" s="1">
+        <v>0.26819999999999999</v>
+      </c>
+      <c r="E8" s="1">
         <v>1.6171</v>
       </c>
-      <c r="F8">
-        <v>0.28439999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F8" s="1">
+        <v>0.28439999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>1.7479</v>
       </c>
-      <c r="D9">
-        <v>0.28439999999999999</v>
-      </c>
-      <c r="E9">
+      <c r="D9" s="1">
+        <v>0.28439999999999999</v>
+      </c>
+      <c r="E9" s="1">
         <v>1.9601999999999999</v>
       </c>
-      <c r="F9">
-        <v>0.28439999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F9" s="1">
+        <v>0.26819999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10">
-        <v>1.7834000000000001</v>
-      </c>
-      <c r="D10">
-        <v>0.26819999999999999</v>
-      </c>
-      <c r="E10">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.7844</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.28439999999999999</v>
+      </c>
+      <c r="E10" s="1">
         <v>1.6171</v>
       </c>
-      <c r="F10">
-        <v>0.28439999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F10" s="1">
+        <v>0.28439999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C11">
-        <v>1.7834000000000001</v>
-      </c>
-      <c r="D11">
-        <v>0.26819999999999999</v>
-      </c>
-      <c r="E11">
+      <c r="C11" s="1">
+        <v>1.7844</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.28439999999999999</v>
+      </c>
+      <c r="E11" s="1">
         <v>1.8615999999999999</v>
       </c>
-      <c r="F11">
-        <v>0.28439999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F11" s="1">
+        <v>0.28439999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>2.0122</v>
       </c>
-      <c r="D12">
-        <v>0.28439999999999999</v>
-      </c>
-      <c r="E12">
+      <c r="D12" s="1">
+        <v>0.26819999999999999</v>
+      </c>
+      <c r="E12" s="1">
         <v>1.9383999999999999</v>
       </c>
-      <c r="F12">
-        <v>0.28439999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F12" s="1">
+        <v>0.28439999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="C13">
-        <v>2.0122</v>
-      </c>
-      <c r="D13">
-        <v>0.28439999999999999</v>
-      </c>
-      <c r="E13">
+      <c r="C13" s="1">
         <v>1.9601999999999999</v>
       </c>
-      <c r="F13">
+      <c r="D13" s="1">
+        <v>0.26819999999999999</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1.9383999999999999</v>
+      </c>
+      <c r="F13" s="1">
         <v>0.28439999999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100837E6128234EC548AB2003B7FFFD7248" ma:contentTypeVersion="13" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7419b1af371792a5c40cd487ec56d45d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a14b51b4-7e98-4bef-bc42-d2f4090b482d" xmlns:ns3="8cb485e5-cd52-454c-b439-58854f8d91fc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1af3f5af933e082306989cc90446d8fb" ns2:_="" ns3:_="">
+    <xsd:import namespace="a14b51b4-7e98-4bef-bc42-d2f4090b482d"/>
+    <xsd:import namespace="8cb485e5-cd52-454c-b439-58854f8d91fc"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceBillingMetadata" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a14b51b4-7e98-4bef-bc42-d2f4090b482d" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="11" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Bildmarkierungen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="7873907d-d049-4c15-acb6-7b8f2d6df672" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="18" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceBillingMetadata" ma:index="20" nillable="true" ma:displayName="MediaServiceBillingMetadata" ma:hidden="true" ma:internalName="MediaServiceBillingMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="8cb485e5-cd52-454c-b439-58854f8d91fc" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="14" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{d39130b4-ab38-41fd-9263-2ff3a96d8917}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="8cb485e5-cd52-454c-b439-58854f8d91fc">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhaltstyp"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="8cb485e5-cd52-454c-b439-58854f8d91fc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a14b51b4-7e98-4bef-bc42-d2f4090b482d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46F83570-8BDF-4A10-B005-B65F89CA8DC7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61453DE8-E289-4F12-8622-E22131B6D1BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a14b51b4-7e98-4bef-bc42-d2f4090b482d"/>
+    <ds:schemaRef ds:uri="8cb485e5-cd52-454c-b439-58854f8d91fc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F73D6A79-6690-45C5-86E5-6F770435DDC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="8cb485e5-cd52-454c-b439-58854f8d91fc"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a14b51b4-7e98-4bef-bc42-d2f4090b482d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>